<commit_message>
adding info to the data so I can filter by location
</commit_message>
<xml_diff>
--- a/data/deep_water_fish_diversity/site.xlsx
+++ b/data/deep_water_fish_diversity/site.xlsx
@@ -1,21 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DEEPFISH\data\report\diversity\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27840" windowHeight="11580"/>
+    <workbookView xWindow="8460" yWindow="2460" windowWidth="27840" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -24,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>site</t>
   </si>
@@ -42,16 +40,38 @@
   </si>
   <si>
     <t>Piggy_Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">location </t>
+  </si>
+  <si>
+    <t>anacapa_island</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,13 +94,49 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="19">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -139,7 +195,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -174,7 +230,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -351,7 +407,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -359,59 +415,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2">
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
         <v>33.991999999999997</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>-119.472666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
         <v>33.956712328767097</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>-119.478493150685</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
         <v>33.917499999999997</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>-119.47750000000001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
plotting average diversity and biomass rather than each data point
</commit_message>
<xml_diff>
--- a/data/deep_water_fish_diversity/site.xlsx
+++ b/data/deep_water_fish_diversity/site.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27127"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8460" yWindow="2460" windowWidth="27840" windowHeight="11220"/>
+    <workbookView xWindow="39680" yWindow="1980" windowWidth="27840" windowHeight="11220"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>site</t>
   </si>
@@ -33,19 +33,25 @@
     <t>long</t>
   </si>
   <si>
-    <t>Anacapa_Passage</t>
-  </si>
-  <si>
     <t>Footprint</t>
   </si>
   <si>
-    <t>Piggy_Bank</t>
-  </si>
-  <si>
     <t xml:space="preserve">location </t>
   </si>
   <si>
-    <t>anacapa_island</t>
+    <t>anacapa_passage</t>
+  </si>
+  <si>
+    <t>footprint</t>
+  </si>
+  <si>
+    <t>piggy_bank</t>
+  </si>
+  <si>
+    <t>Anacapa Passage</t>
+  </si>
+  <si>
+    <t>Piggy Bank</t>
   </si>
 </sst>
 </file>
@@ -94,8 +100,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -118,7 +126,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -128,6 +136,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -137,6 +146,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -418,7 +428,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -428,7 +438,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -439,10 +449,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>33.991999999999997</v>
@@ -453,10 +463,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3">
         <v>33.956712328767097</v>
@@ -467,7 +477,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Add locations to deep water fish
</commit_message>
<xml_diff>
--- a/data/deep_water_fish_diversity/site.xlsx
+++ b/data/deep_water_fish_diversity/site.xlsx
@@ -428,10 +428,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">

</xml_diff>